<commit_message>
Add sd to Programa
</commit_message>
<xml_diff>
--- a/Files/DATA.xlsx
+++ b/Files/DATA.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Indra\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB705760-42AC-4752-BBBB-E58D4A582F72}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
     <sheet name="CALCULO" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="120">
   <si>
     <t>PROYECTO 01</t>
   </si>
@@ -383,12 +382,21 @@
   </si>
   <si>
     <t>Fecha</t>
+  </si>
+  <si>
+    <t>Herramienta interactiva de visualización de datos para la Web</t>
+  </si>
+  <si>
+    <t>Se propone el desarrollo de una herramienta interactiva de visualización de datos que haga uso de las facilidades ofrecidas por HTML5, sin recurrir al uso de plug-ins externos (Flash, Java). NOTA: En http://www.chromeexperiments.com se pueden ver algunos ejemplos de lo que se puede conseguir utilizando exclusivamente HTML, CSS y JavaScript.</t>
+  </si>
+  <si>
+    <t>PY-2018-08-00004</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -649,6 +657,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -664,13 +674,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -947,40 +955,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:W37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:W63"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59:J62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.73046875" customWidth="1"/>
-    <col min="2" max="2" width="20.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.73046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="45.265625" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="255.73046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>40</v>
       </c>
@@ -1000,14 +1008,14 @@
       <c r="I1" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="42"/>
-    </row>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.45">
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="44"/>
+    </row>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>41</v>
       </c>
@@ -1040,7 +1048,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E3" s="21" t="s">
         <v>44</v>
       </c>
@@ -1069,7 +1077,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E4" s="21" t="s">
         <v>45</v>
       </c>
@@ -1096,7 +1104,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E5" s="21" t="s">
         <v>46</v>
       </c>
@@ -1119,7 +1127,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="2:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6" s="26" t="s">
         <v>47</v>
       </c>
@@ -1140,7 +1148,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="J7" s="21">
         <v>5</v>
       </c>
@@ -1154,7 +1162,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="2:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="J8" s="21">
         <v>6</v>
       </c>
@@ -1168,7 +1176,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="2:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="J9" s="21">
         <v>7</v>
       </c>
@@ -1182,7 +1190,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="J10" s="21">
         <v>8</v>
       </c>
@@ -1196,7 +1204,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="J11" s="21">
         <v>9</v>
       </c>
@@ -1210,7 +1218,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:20" s="17" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="J12" s="21">
         <v>10</v>
       </c>
@@ -1224,7 +1232,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:20" s="17" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:20" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J13" s="26">
         <v>11</v>
       </c>
@@ -1238,9 +1246,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="2:20" s="17" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="15" spans="2:20" s="17" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:20" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:20" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="H16" s="7" t="s">
         <v>64</v>
       </c>
@@ -1251,7 +1259,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>37</v>
       </c>
@@ -1319,7 +1327,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C18" s="5">
         <v>1</v>
       </c>
@@ -1390,12 +1398,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
       <c r="J20" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>11</v>
       </c>
@@ -1436,7 +1444,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C22" s="5">
         <v>1</v>
       </c>
@@ -1467,6 +1475,7 @@
         <v>2</v>
       </c>
       <c r="L22" s="5">
+        <f>$C$18</f>
         <v>1</v>
       </c>
       <c r="M22" s="14">
@@ -1478,7 +1487,7 @@
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C23" s="5">
         <v>2</v>
       </c>
@@ -1509,6 +1518,7 @@
         <v>3</v>
       </c>
       <c r="L23" s="5">
+        <f t="shared" ref="L23:L26" si="1">$C$18</f>
         <v>1</v>
       </c>
       <c r="M23" s="14">
@@ -1516,11 +1526,11 @@
         <v>0.13333333333333333</v>
       </c>
       <c r="N23" s="14">
-        <f t="shared" ref="N23:N26" si="1">IF(J23=2,M23/100,0)</f>
+        <f t="shared" ref="N23:N26" si="2">IF(J23=2,M23/100,0)</f>
         <v>1.3333333333333333E-3</v>
       </c>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C24" s="5">
         <v>3</v>
       </c>
@@ -1537,7 +1547,7 @@
         <v>3</v>
       </c>
       <c r="H24" s="6">
-        <f t="shared" ref="H24:H26" si="2">I23</f>
+        <f t="shared" ref="H24:H26" si="3">I23</f>
         <v>43342</v>
       </c>
       <c r="I24" s="6">
@@ -1551,18 +1561,19 @@
         <v>4</v>
       </c>
       <c r="L24" s="5">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M24" s="14">
-        <f t="shared" ref="M23:M26" si="3">G24/$T$18</f>
+        <f t="shared" ref="M24:M26" si="4">G24/$T$18</f>
         <v>0.2</v>
       </c>
       <c r="N24" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C25" s="5">
         <v>4</v>
       </c>
@@ -1579,7 +1590,7 @@
         <v>4</v>
       </c>
       <c r="H25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43345</v>
       </c>
       <c r="I25" s="6">
@@ -1593,18 +1604,19 @@
         <v>5</v>
       </c>
       <c r="L25" s="5">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M25" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.26666666666666666</v>
       </c>
       <c r="N25" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C26" s="5">
         <v>5</v>
       </c>
@@ -1621,7 +1633,7 @@
         <v>5</v>
       </c>
       <c r="H26" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43349</v>
       </c>
       <c r="I26" s="6">
@@ -1635,18 +1647,19 @@
         <v>6</v>
       </c>
       <c r="L26" s="5">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M26" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="N26" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C27" s="5"/>
       <c r="D27" s="1"/>
       <c r="E27" s="5"/>
@@ -1660,13 +1673,13 @@
       <c r="M27" s="14"/>
       <c r="N27" s="14"/>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="G28" s="8" t="s">
         <v>72</v>
       </c>
       <c r="N28" s="15"/>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>32</v>
       </c>
@@ -1692,28 +1705,31 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C30" s="5">
         <v>1</v>
       </c>
       <c r="D30" s="5">
+        <f>$C$18</f>
         <v>1</v>
       </c>
       <c r="E30" s="9">
-        <v>43313</v>
+        <f>G18</f>
+        <v>43339</v>
       </c>
       <c r="F30" s="5">
-        <v>3</v>
+        <f>$J$18</f>
+        <v>1</v>
       </c>
       <c r="G30" s="5">
         <v>4</v>
       </c>
       <c r="H30" s="5">
-        <f>N18</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.45">
+        <f>$N$18</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="9"/>
@@ -1721,12 +1737,12 @@
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="J32" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>73</v>
       </c>
@@ -1755,11 +1771,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34">
+        <f>$C$30</f>
         <v>1</v>
       </c>
       <c r="E34">
@@ -1782,11 +1799,12 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>2</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="17">
+        <f t="shared" ref="D35:D37" si="5">$C$30</f>
         <v>1</v>
       </c>
       <c r="E35">
@@ -1809,11 +1827,12 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>3</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="17">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="E36">
@@ -1836,11 +1855,12 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>4</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="17">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="E37">
@@ -1862,54 +1882,1002 @@
         <f>(F37*L10)</f>
         <v>25</v>
       </c>
+    </row>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+      <c r="O41" s="17"/>
+      <c r="P41" s="17"/>
+      <c r="Q41" s="17"/>
+      <c r="R41" s="17"/>
+      <c r="S41" s="17"/>
+      <c r="T41" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="U41" s="17"/>
+      <c r="V41" s="17"/>
+      <c r="W41" s="17"/>
+    </row>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B42" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K42" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="L42" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="M42" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="N42" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="O42" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="P42" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q42" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="R42" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="S42" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="T42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U42" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="V42" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="W42" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B43" s="17"/>
+      <c r="C43" s="5">
+        <v>4</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" s="13">
+        <v>7000</v>
+      </c>
+      <c r="F43" s="2">
+        <f>SUM(J59:J62)</f>
+        <v>6800</v>
+      </c>
+      <c r="G43" s="9">
+        <v>43327</v>
+      </c>
+      <c r="H43" s="6">
+        <f>I51</f>
+        <v>43345</v>
+      </c>
+      <c r="I43" s="10">
+        <v>2</v>
+      </c>
+      <c r="J43" s="5">
+        <v>3</v>
+      </c>
+      <c r="K43" s="5">
+        <v>1</v>
+      </c>
+      <c r="L43" s="5">
+        <v>1</v>
+      </c>
+      <c r="M43" s="5">
+        <v>2</v>
+      </c>
+      <c r="N43" s="5">
+        <v>1</v>
+      </c>
+      <c r="O43" s="5">
+        <v>1</v>
+      </c>
+      <c r="P43" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q43" s="9">
+        <f>G43</f>
+        <v>43327</v>
+      </c>
+      <c r="R43" s="9">
+        <f>Q43</f>
+        <v>43327</v>
+      </c>
+      <c r="S43" s="10">
+        <v>1</v>
+      </c>
+      <c r="T43" s="12">
+        <f>SUM(G47:G51)</f>
+        <v>18</v>
+      </c>
+      <c r="U43" s="16">
+        <f>SUM(N47:N51)</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="V43" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W43" s="17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="17"/>
+      <c r="M44" s="17"/>
+      <c r="N44" s="17"/>
+      <c r="O44" s="17"/>
+      <c r="P44" s="17"/>
+      <c r="Q44" s="17"/>
+      <c r="R44" s="17"/>
+      <c r="S44" s="17"/>
+      <c r="T44" s="17"/>
+      <c r="U44" s="17"/>
+      <c r="V44" s="17"/>
+      <c r="W44" s="17"/>
+    </row>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K45" s="17"/>
+      <c r="L45" s="17"/>
+      <c r="M45" s="17"/>
+      <c r="N45" s="17"/>
+      <c r="O45" s="17"/>
+      <c r="P45" s="17"/>
+      <c r="Q45" s="17"/>
+      <c r="R45" s="17"/>
+      <c r="S45" s="17"/>
+      <c r="T45" s="17"/>
+      <c r="U45" s="17"/>
+      <c r="V45" s="17"/>
+      <c r="W45" s="17"/>
+    </row>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B46" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G46" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J46" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="K46" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L46" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="M46" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="N46" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O46" s="17"/>
+      <c r="P46" s="17"/>
+      <c r="Q46" s="17"/>
+      <c r="R46" s="17"/>
+      <c r="S46" s="17"/>
+      <c r="T46" s="17"/>
+      <c r="U46" s="17"/>
+      <c r="V46" s="17"/>
+      <c r="W46" s="17"/>
+    </row>
+    <row r="47" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B47" s="17"/>
+      <c r="C47" s="5">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E47" s="5">
+        <v>1</v>
+      </c>
+      <c r="F47" s="10">
+        <v>1</v>
+      </c>
+      <c r="G47" s="5">
+        <v>1</v>
+      </c>
+      <c r="H47" s="6">
+        <f>G43</f>
+        <v>43327</v>
+      </c>
+      <c r="I47" s="6">
+        <f>H47+G47</f>
+        <v>43328</v>
+      </c>
+      <c r="J47" s="5">
+        <v>2</v>
+      </c>
+      <c r="K47" s="5">
+        <v>2</v>
+      </c>
+      <c r="L47" s="5">
+        <f>$C$43</f>
+        <v>4</v>
+      </c>
+      <c r="M47" s="14">
+        <f>(G47/$T$43)</f>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="N47" s="14">
+        <f>IF(J47=2,M47,0)</f>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="O47" s="17"/>
+      <c r="P47" s="17"/>
+      <c r="Q47" s="17"/>
+      <c r="R47" s="17"/>
+      <c r="S47" s="17"/>
+      <c r="T47" s="17"/>
+      <c r="U47" s="17"/>
+      <c r="V47" s="17"/>
+      <c r="W47" s="17"/>
+    </row>
+    <row r="48" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B48" s="17"/>
+      <c r="C48" s="5">
+        <v>2</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E48" s="5">
+        <v>2</v>
+      </c>
+      <c r="F48" s="10">
+        <v>1</v>
+      </c>
+      <c r="G48" s="5">
+        <v>3</v>
+      </c>
+      <c r="H48" s="6">
+        <f>I47</f>
+        <v>43328</v>
+      </c>
+      <c r="I48" s="6">
+        <f t="shared" ref="I48:I51" si="6">H48+G48</f>
+        <v>43331</v>
+      </c>
+      <c r="J48" s="5">
+        <v>2</v>
+      </c>
+      <c r="K48" s="5">
+        <v>3</v>
+      </c>
+      <c r="L48" s="5">
+        <f t="shared" ref="L48:L51" si="7">$C$43</f>
+        <v>4</v>
+      </c>
+      <c r="M48" s="14">
+        <f t="shared" ref="M48:M51" si="8">(G48/$T$43)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="N48" s="14">
+        <f t="shared" ref="N48:N51" si="9">IF(J48=2,M48,0)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="O48" s="17"/>
+      <c r="P48" s="17"/>
+      <c r="Q48" s="17"/>
+      <c r="R48" s="17"/>
+      <c r="S48" s="17"/>
+      <c r="T48" s="17"/>
+      <c r="U48" s="17"/>
+      <c r="V48" s="17"/>
+      <c r="W48" s="17"/>
+    </row>
+    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B49" s="17"/>
+      <c r="C49" s="5">
+        <v>3</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E49" s="5">
+        <v>3</v>
+      </c>
+      <c r="F49" s="10">
+        <v>1</v>
+      </c>
+      <c r="G49" s="5">
+        <v>4</v>
+      </c>
+      <c r="H49" s="6">
+        <f t="shared" ref="H49:H51" si="10">I48</f>
+        <v>43331</v>
+      </c>
+      <c r="I49" s="6">
+        <f t="shared" si="6"/>
+        <v>43335</v>
+      </c>
+      <c r="J49" s="5">
+        <v>3</v>
+      </c>
+      <c r="K49" s="5">
+        <v>4</v>
+      </c>
+      <c r="L49" s="5">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="M49" s="14">
+        <f t="shared" si="8"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="N49" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O49" s="17"/>
+      <c r="P49" s="17"/>
+      <c r="Q49" s="17"/>
+      <c r="R49" s="17"/>
+      <c r="S49" s="17"/>
+      <c r="T49" s="17"/>
+      <c r="U49" s="17"/>
+      <c r="V49" s="17"/>
+      <c r="W49" s="17"/>
+    </row>
+    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B50" s="17"/>
+      <c r="C50" s="5">
+        <v>4</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E50" s="5">
+        <v>4</v>
+      </c>
+      <c r="F50" s="10">
+        <v>1</v>
+      </c>
+      <c r="G50" s="5">
+        <v>8</v>
+      </c>
+      <c r="H50" s="6">
+        <f t="shared" si="10"/>
+        <v>43335</v>
+      </c>
+      <c r="I50" s="6">
+        <f t="shared" si="6"/>
+        <v>43343</v>
+      </c>
+      <c r="J50" s="5">
+        <v>3</v>
+      </c>
+      <c r="K50" s="5">
+        <v>5</v>
+      </c>
+      <c r="L50" s="5">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="M50" s="14">
+        <f t="shared" si="8"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="N50" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
+      <c r="Q50" s="17"/>
+      <c r="R50" s="17"/>
+      <c r="S50" s="17"/>
+      <c r="T50" s="17"/>
+      <c r="U50" s="17"/>
+      <c r="V50" s="17"/>
+      <c r="W50" s="17"/>
+    </row>
+    <row r="51" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B51" s="17"/>
+      <c r="C51" s="5">
+        <v>5</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E51" s="5">
+        <v>5</v>
+      </c>
+      <c r="F51" s="10">
+        <v>1</v>
+      </c>
+      <c r="G51" s="5">
+        <v>2</v>
+      </c>
+      <c r="H51" s="6">
+        <f t="shared" si="10"/>
+        <v>43343</v>
+      </c>
+      <c r="I51" s="6">
+        <f t="shared" si="6"/>
+        <v>43345</v>
+      </c>
+      <c r="J51" s="5">
+        <v>3</v>
+      </c>
+      <c r="K51" s="5">
+        <v>6</v>
+      </c>
+      <c r="L51" s="5">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="M51" s="14">
+        <f t="shared" si="8"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="N51" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O51" s="17"/>
+      <c r="P51" s="17"/>
+      <c r="Q51" s="17"/>
+      <c r="R51" s="17"/>
+      <c r="S51" s="17"/>
+      <c r="T51" s="17"/>
+      <c r="U51" s="17"/>
+      <c r="V51" s="17"/>
+      <c r="W51" s="17"/>
+    </row>
+    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B52" s="17"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="14"/>
+      <c r="N52" s="14"/>
+      <c r="O52" s="17"/>
+      <c r="P52" s="17"/>
+      <c r="Q52" s="17"/>
+      <c r="R52" s="17"/>
+      <c r="S52" s="17"/>
+      <c r="T52" s="17"/>
+      <c r="U52" s="17"/>
+      <c r="V52" s="17"/>
+      <c r="W52" s="17"/>
+    </row>
+    <row r="53" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B53" s="17"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="17"/>
+      <c r="L53" s="17"/>
+      <c r="M53" s="17"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="17"/>
+      <c r="P53" s="17"/>
+      <c r="Q53" s="17"/>
+      <c r="R53" s="17"/>
+      <c r="S53" s="17"/>
+      <c r="T53" s="17"/>
+      <c r="U53" s="17"/>
+      <c r="V53" s="17"/>
+      <c r="W53" s="17"/>
+    </row>
+    <row r="54" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B54" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G54" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H54" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="I54" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="J54" s="17"/>
+      <c r="K54" s="17"/>
+      <c r="L54" s="17"/>
+      <c r="M54" s="17"/>
+      <c r="N54" s="17"/>
+      <c r="O54" s="17"/>
+      <c r="P54" s="17"/>
+      <c r="Q54" s="17"/>
+      <c r="R54" s="17"/>
+      <c r="S54" s="17"/>
+      <c r="T54" s="17"/>
+      <c r="U54" s="17"/>
+      <c r="V54" s="17"/>
+      <c r="W54" s="17"/>
+    </row>
+    <row r="55" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B55" s="17"/>
+      <c r="C55" s="5">
+        <v>4</v>
+      </c>
+      <c r="D55" s="5">
+        <v>4</v>
+      </c>
+      <c r="E55" s="9">
+        <f>$G$43</f>
+        <v>43327</v>
+      </c>
+      <c r="F55" s="5">
+        <f>$J$43</f>
+        <v>3</v>
+      </c>
+      <c r="G55" s="5">
+        <v>4</v>
+      </c>
+      <c r="H55" s="5">
+        <v>1</v>
+      </c>
+      <c r="I55" s="17"/>
+      <c r="J55" s="17"/>
+      <c r="K55" s="17"/>
+      <c r="L55" s="17"/>
+      <c r="M55" s="17"/>
+      <c r="N55" s="17"/>
+      <c r="O55" s="17"/>
+      <c r="P55" s="17"/>
+      <c r="Q55" s="17"/>
+      <c r="R55" s="17"/>
+      <c r="S55" s="17"/>
+      <c r="T55" s="17"/>
+      <c r="U55" s="17"/>
+      <c r="V55" s="17"/>
+      <c r="W55" s="17"/>
+    </row>
+    <row r="56" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B56" s="17"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="17"/>
+      <c r="O56" s="17"/>
+      <c r="P56" s="17"/>
+      <c r="Q56" s="17"/>
+      <c r="R56" s="17"/>
+      <c r="S56" s="17"/>
+      <c r="T56" s="17"/>
+      <c r="U56" s="17"/>
+      <c r="V56" s="17"/>
+      <c r="W56" s="17"/>
+    </row>
+    <row r="57" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B57" s="17"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="17"/>
+      <c r="J57" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K57" s="17"/>
+      <c r="L57" s="17"/>
+      <c r="M57" s="17"/>
+      <c r="N57" s="17"/>
+      <c r="O57" s="17"/>
+      <c r="P57" s="17"/>
+      <c r="Q57" s="17"/>
+      <c r="R57" s="17"/>
+      <c r="S57" s="17"/>
+      <c r="T57" s="17"/>
+      <c r="U57" s="17"/>
+      <c r="V57" s="17"/>
+      <c r="W57" s="17"/>
+    </row>
+    <row r="58" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B58" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E58" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G58" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="H58" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="I58" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K58" s="17"/>
+      <c r="L58" s="17"/>
+      <c r="M58" s="17"/>
+      <c r="N58" s="17"/>
+      <c r="O58" s="17"/>
+      <c r="P58" s="17"/>
+      <c r="Q58" s="17"/>
+      <c r="R58" s="17"/>
+      <c r="S58" s="17"/>
+      <c r="T58" s="17"/>
+      <c r="U58" s="17"/>
+      <c r="V58" s="17"/>
+      <c r="W58" s="17"/>
+    </row>
+    <row r="59" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B59" s="17"/>
+      <c r="C59" s="17">
+        <v>1</v>
+      </c>
+      <c r="D59" s="17">
+        <f>$C$55</f>
+        <v>4</v>
+      </c>
+      <c r="E59" s="17">
+        <v>1</v>
+      </c>
+      <c r="F59" s="17">
+        <v>2</v>
+      </c>
+      <c r="G59" s="17">
+        <v>6</v>
+      </c>
+      <c r="H59" s="17">
+        <v>2</v>
+      </c>
+      <c r="I59" s="17">
+        <v>18</v>
+      </c>
+      <c r="J59" s="2">
+        <f>(F59*M3)*I59</f>
+        <v>1800</v>
+      </c>
+      <c r="K59" s="17"/>
+      <c r="L59" s="17"/>
+      <c r="M59" s="17"/>
+      <c r="N59" s="17"/>
+      <c r="O59" s="17"/>
+      <c r="P59" s="17"/>
+      <c r="Q59" s="17"/>
+      <c r="R59" s="17"/>
+      <c r="S59" s="17"/>
+      <c r="T59" s="17"/>
+      <c r="U59" s="17"/>
+      <c r="V59" s="17"/>
+      <c r="W59" s="17"/>
+    </row>
+    <row r="60" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B60" s="17"/>
+      <c r="C60" s="17">
+        <v>2</v>
+      </c>
+      <c r="D60" s="17">
+        <f t="shared" ref="D60:D62" si="11">$C$55</f>
+        <v>4</v>
+      </c>
+      <c r="E60" s="17">
+        <v>3</v>
+      </c>
+      <c r="F60" s="17">
+        <v>4</v>
+      </c>
+      <c r="G60" s="17">
+        <v>3</v>
+      </c>
+      <c r="H60" s="17">
+        <v>2</v>
+      </c>
+      <c r="I60" s="17">
+        <v>18</v>
+      </c>
+      <c r="J60" s="2">
+        <f>(F60*M5)*I60</f>
+        <v>3600</v>
+      </c>
+      <c r="K60" s="17"/>
+      <c r="L60" s="17"/>
+      <c r="M60" s="17"/>
+      <c r="N60" s="17"/>
+      <c r="O60" s="17"/>
+      <c r="P60" s="17"/>
+      <c r="Q60" s="17"/>
+      <c r="R60" s="17"/>
+      <c r="S60" s="17"/>
+      <c r="T60" s="17"/>
+      <c r="U60" s="17"/>
+      <c r="V60" s="17"/>
+      <c r="W60" s="17"/>
+    </row>
+    <row r="61" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B61" s="17"/>
+      <c r="C61" s="17">
+        <v>3</v>
+      </c>
+      <c r="D61" s="17">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="E61" s="17">
+        <v>9</v>
+      </c>
+      <c r="F61" s="17">
+        <v>5</v>
+      </c>
+      <c r="G61" s="17">
+        <v>6</v>
+      </c>
+      <c r="H61" s="17">
+        <v>2</v>
+      </c>
+      <c r="I61" s="17">
+        <v>18</v>
+      </c>
+      <c r="J61" s="2">
+        <f>(F61*M11)*I61</f>
+        <v>1350</v>
+      </c>
+      <c r="K61" s="17"/>
+      <c r="L61" s="17"/>
+      <c r="M61" s="17"/>
+      <c r="N61" s="17"/>
+      <c r="O61" s="17"/>
+      <c r="P61" s="17"/>
+      <c r="Q61" s="17"/>
+      <c r="R61" s="17"/>
+      <c r="S61" s="17"/>
+      <c r="T61" s="17"/>
+      <c r="U61" s="17"/>
+      <c r="V61" s="17"/>
+      <c r="W61" s="17"/>
+    </row>
+    <row r="62" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B62" s="17"/>
+      <c r="C62" s="17">
+        <v>4</v>
+      </c>
+      <c r="D62" s="17">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="E62" s="17">
+        <v>8</v>
+      </c>
+      <c r="F62" s="17">
+        <v>2</v>
+      </c>
+      <c r="G62" s="17">
+        <v>2</v>
+      </c>
+      <c r="H62" s="17">
+        <v>1</v>
+      </c>
+      <c r="I62" s="17">
+        <v>0</v>
+      </c>
+      <c r="J62" s="2">
+        <f>(F62*L10)</f>
+        <v>50</v>
+      </c>
+      <c r="K62" s="17"/>
+      <c r="L62" s="17"/>
+      <c r="M62" s="17"/>
+      <c r="N62" s="17"/>
+      <c r="O62" s="17"/>
+      <c r="P62" s="17"/>
+      <c r="Q62" s="17"/>
+      <c r="R62" s="17"/>
+      <c r="S62" s="17"/>
+      <c r="T62" s="17"/>
+      <c r="U62" s="17"/>
+      <c r="V62" s="17"/>
+      <c r="W62" s="17"/>
+    </row>
+    <row r="63" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="17"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
+      <c r="M63" s="17"/>
+      <c r="N63" s="17"/>
+      <c r="O63" s="17"/>
+      <c r="P63" s="17"/>
+      <c r="Q63" s="17"/>
+      <c r="R63" s="17"/>
+      <c r="S63" s="17"/>
+      <c r="T63" s="17"/>
+      <c r="U63" s="17"/>
+      <c r="V63" s="17"/>
+      <c r="W63" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="J1:M1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="P18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="P18" r:id="rId1"/>
+    <hyperlink ref="P43" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05B110A-C7E2-49F6-9721-18A509992D20}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.06640625" style="17"/>
-    <col min="6" max="6" width="10.19921875" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="17"/>
+    <col min="6" max="6" width="10.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="45">
+      <c r="C1" s="40">
         <f>SUM(B5:B9)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="45">
+      <c r="C2" s="40">
         <f>SUM(E5:E9)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
         <v>30</v>
       </c>
@@ -1932,137 +2900,137 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="45">
+      <c r="C5" s="40">
         <f>(B5/$C$1)*100</f>
         <v>6.666666666666667</v>
       </c>
       <c r="D5" s="5">
         <v>2</v>
       </c>
-      <c r="E5" s="45">
+      <c r="E5" s="40">
         <f>IF(D5=2,C5,0)</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="F5" s="46">
+      <c r="F5" s="41">
         <v>43340</v>
       </c>
-      <c r="G5" s="45">
+      <c r="G5" s="40">
         <f>C5</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="H5" s="45">
+      <c r="H5" s="40">
         <f>E5</f>
         <v>6.666666666666667</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>2</v>
       </c>
-      <c r="C6" s="45">
+      <c r="C6" s="40">
         <f t="shared" ref="C6:C9" si="0">(B6/$C$1)*100</f>
         <v>13.333333333333334</v>
       </c>
       <c r="D6" s="5">
         <v>2</v>
       </c>
-      <c r="E6" s="45">
+      <c r="E6" s="40">
         <f t="shared" ref="E6:E9" si="1">IF(D6=2,C6,0)</f>
         <v>13.333333333333334</v>
       </c>
-      <c r="F6" s="46">
+      <c r="F6" s="41">
         <v>43342</v>
       </c>
-      <c r="G6" s="45">
+      <c r="G6" s="40">
         <f>G5+C6</f>
         <v>20</v>
       </c>
-      <c r="H6" s="45">
+      <c r="H6" s="40">
         <f>H5+E6</f>
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>3</v>
       </c>
-      <c r="C7" s="45">
+      <c r="C7" s="40">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="D7" s="5">
         <v>3</v>
       </c>
-      <c r="E7" s="45">
+      <c r="E7" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F7" s="46">
+      <c r="F7" s="41">
         <v>43345</v>
       </c>
-      <c r="G7" s="45">
+      <c r="G7" s="40">
         <f t="shared" ref="G7:G9" si="2">G6+C7</f>
         <v>40</v>
       </c>
-      <c r="H7" s="45">
+      <c r="H7" s="40">
         <f t="shared" ref="H7:H9" si="3">H6+E7</f>
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>4</v>
       </c>
-      <c r="C8" s="45">
+      <c r="C8" s="40">
         <f t="shared" si="0"/>
         <v>26.666666666666668</v>
       </c>
       <c r="D8" s="5">
         <v>3</v>
       </c>
-      <c r="E8" s="45">
+      <c r="E8" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8" s="46">
+      <c r="F8" s="41">
         <v>43349</v>
       </c>
-      <c r="G8" s="45">
+      <c r="G8" s="40">
         <f t="shared" si="2"/>
         <v>66.666666666666671</v>
       </c>
-      <c r="H8" s="45">
+      <c r="H8" s="40">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>5</v>
       </c>
-      <c r="C9" s="45">
+      <c r="C9" s="40">
         <f t="shared" si="0"/>
         <v>33.333333333333329</v>
       </c>
       <c r="D9" s="5">
         <v>3</v>
       </c>
-      <c r="E9" s="45">
+      <c r="E9" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F9" s="46">
+      <c r="F9" s="41">
         <v>43354</v>
       </c>
-      <c r="G9" s="45">
+      <c r="G9" s="40">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="H9" s="45">
+      <c r="H9" s="40">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
@@ -2074,24 +3042,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B2" s="43" t="s">
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="44"/>
+      <c r="C2" s="46"/>
       <c r="D2" s="18" t="s">
         <v>86</v>
       </c>
@@ -2105,7 +3073,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
         <v>0</v>
       </c>
@@ -2123,7 +3091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="21"/>
       <c r="C4" s="22" t="s">
         <v>1</v>
@@ -2143,7 +3111,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="21"/>
       <c r="C5" s="22" t="s">
         <v>2</v>
@@ -2163,7 +3131,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="21"/>
       <c r="C6" s="22" t="s">
         <v>3</v>
@@ -2183,7 +3151,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="21"/>
       <c r="C7" s="22" t="s">
         <v>4</v>
@@ -2203,7 +3171,7 @@
         <v>0.20833333333333334</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="21"/>
       <c r="C8" s="22" t="s">
         <v>5</v>
@@ -2223,7 +3191,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="21"/>
       <c r="C9" s="22" t="s">
         <v>6</v>
@@ -2243,7 +3211,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="21"/>
       <c r="C10" s="22" t="s">
         <v>7</v>
@@ -2263,7 +3231,7 @@
         <v>9.5833333333333326E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
       <c r="C11" s="22" t="s">
         <v>8</v>
@@ -2283,7 +3251,7 @@
         <v>7.0833333333333331E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="21"/>
       <c r="C12" s="22" t="s">
         <v>9</v>
@@ -2303,7 +3271,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="26"/>
       <c r="C13" s="27" t="s">
         <v>10</v>
@@ -2323,7 +3291,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -2331,11 +3299,11 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B15" s="43" t="s">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="C15" s="44"/>
+      <c r="C15" s="46"/>
       <c r="D15" s="18" t="s">
         <v>86</v>
       </c>
@@ -2349,7 +3317,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="21" t="s">
         <v>91</v>
       </c>
@@ -2367,7 +3335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="21"/>
       <c r="C17" s="22" t="s">
         <v>92</v>
@@ -2387,7 +3355,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="21"/>
       <c r="C18" s="22" t="s">
         <v>93</v>
@@ -2407,7 +3375,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="21"/>
       <c r="C19" s="22" t="s">
         <v>94</v>
@@ -2427,7 +3395,7 @@
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="21"/>
       <c r="C20" s="22" t="s">
         <v>95</v>
@@ -2447,7 +3415,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="21"/>
       <c r="C21" s="22" t="s">
         <v>96</v>
@@ -2467,7 +3435,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="26"/>
       <c r="C22" s="27" t="s">
         <v>97</v>

</xml_diff>

<commit_message>
add sd to portafolio
</commit_message>
<xml_diff>
--- a/Files/DATA.xlsx
+++ b/Files/DATA.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="124">
   <si>
     <t>PROYECTO 01</t>
   </si>
@@ -132,15 +132,6 @@
     <t>SOLICITUDES</t>
   </si>
   <si>
-    <t>PY-2018-08-00001</t>
-  </si>
-  <si>
-    <t>Software para el diseño de redes de ordenadores</t>
-  </si>
-  <si>
-    <t>El diseño asistido por ordenador, más conocido como CAD (computer-aided design), es el uso de un amplio rango de herramientas computacionales que asisten a ingenieros, arquitectos y a otros profesionales del diseño en sus respectivas actividades. En este proyecto se creara una pequeña herramienta CAD que permita diseñar redes de ordenadores basicas de diferentes clases (e.g., Ethernet, FDDI). El software permitira crear redes virtuales utilizando iconos descriptivos que representen diferentes ordenadores, tarjetas de red, cables y routers, entre otros. Esta herramienta asistira a estudiantes de otras titulaciones a la hora de comprender los conceptos basicos del diseño de redes de una forma amigable.</t>
-  </si>
-  <si>
     <t>admin@indra.com</t>
   </si>
   <si>
@@ -391,6 +382,27 @@
   </si>
   <si>
     <t>PY-2018-08-00004</t>
+  </si>
+  <si>
+    <t>[1/2/3/4]</t>
+  </si>
+  <si>
+    <t>[1…28]</t>
+  </si>
+  <si>
+    <t>[1...22]</t>
+  </si>
+  <si>
+    <t>PY-2018-08-00006</t>
+  </si>
+  <si>
+    <t>[1/2/3]</t>
+  </si>
+  <si>
+    <t>Diseño y desarrollo de un Tutor Inteligente</t>
+  </si>
+  <si>
+    <t>Se pretende desarrollar un sistema de e-learning que incorpore un tutor inteligente que adapte el material docente a las necesidades individuales del alumno.</t>
   </si>
 </sst>
 </file>
@@ -958,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59:J62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,26 +1002,26 @@
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2"/>
       <c r="E1" s="35" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H1" s="36" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I1" s="36" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J1" s="42" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K1" s="43"/>
       <c r="L1" s="43"/>
@@ -1017,23 +1029,23 @@
     </row>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" s="3"/>
       <c r="E2" s="21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H2" s="39" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I2" s="39" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J2" s="31" t="s">
         <v>13</v>
@@ -1042,33 +1054,33 @@
         <v>14</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M2" s="32" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E3" s="21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G3" s="37" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H3" s="39" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I3" s="39" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J3" s="21">
         <v>1</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="L3" s="22">
         <v>3000</v>
@@ -1079,23 +1091,23 @@
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E4" s="21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G4" s="37" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H4" s="37" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I4" s="37"/>
       <c r="J4" s="21">
         <v>2</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="L4" s="22">
         <v>300</v>
@@ -1106,19 +1118,19 @@
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E5" s="21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
       <c r="H5" s="37" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I5" s="37"/>
       <c r="J5" s="21">
         <v>3</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="L5" s="22">
         <v>300</v>
@@ -1129,7 +1141,7 @@
     </row>
     <row r="6" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6" s="26" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F6" s="38"/>
       <c r="G6" s="38"/>
@@ -1139,7 +1151,7 @@
         <v>4</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="L6" s="22">
         <v>100</v>
@@ -1153,7 +1165,7 @@
         <v>5</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L7" s="22">
         <v>48750</v>
@@ -1167,7 +1179,7 @@
         <v>6</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L8" s="22">
         <v>65000</v>
@@ -1181,7 +1193,7 @@
         <v>7</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L9" s="22">
         <v>100</v>
@@ -1195,7 +1207,7 @@
         <v>8</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="L10" s="22">
         <v>25</v>
@@ -1209,7 +1221,7 @@
         <v>9</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="L11" s="22">
         <v>300</v>
@@ -1223,7 +1235,7 @@
         <v>10</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L12" s="22">
         <v>500</v>
@@ -1237,7 +1249,7 @@
         <v>11</v>
       </c>
       <c r="K13" s="27" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="L13" s="27">
         <v>3000</v>
@@ -1250,18 +1262,33 @@
     <row r="15" spans="2:20" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="H16" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>121</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="T16" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
@@ -1273,7 +1300,7 @@
         <v>16</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G17" t="s">
         <v>17</v>
@@ -1329,24 +1356,24 @@
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C18" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>33</v>
+        <v>120</v>
       </c>
       <c r="E18" s="13">
-        <v>8500</v>
+        <v>5650</v>
       </c>
       <c r="F18" s="2">
         <f>SUM(J34:J37)</f>
-        <v>8125</v>
+        <v>5650</v>
       </c>
       <c r="G18" s="9">
-        <v>43339</v>
+        <v>43318</v>
       </c>
       <c r="H18" s="6">
         <f>I26</f>
-        <v>43354</v>
+        <v>43333</v>
       </c>
       <c r="I18" s="10">
         <v>2</v>
@@ -1355,30 +1382,30 @@
         <v>1</v>
       </c>
       <c r="K18" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L18" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M18" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N18" s="5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="O18" s="5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="P18" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="Q18" s="9">
         <f>G18</f>
-        <v>43339</v>
+        <v>43318</v>
       </c>
       <c r="R18" s="9">
         <f>Q18</f>
-        <v>43339</v>
+        <v>43318</v>
       </c>
       <c r="S18" s="10">
         <v>1</v>
@@ -1389,18 +1416,21 @@
       </c>
       <c r="U18" s="16">
         <f>SUM(N22:N26)</f>
-        <v>6.8000000000000005E-2</v>
+        <v>0.01</v>
       </c>
       <c r="V18" t="s">
-        <v>34</v>
+        <v>122</v>
       </c>
       <c r="W18" t="s">
-        <v>35</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.25">
       <c r="J20" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.25">
@@ -1414,7 +1444,7 @@
         <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>29</v>
@@ -1435,10 +1465,10 @@
         <v>24</v>
       </c>
       <c r="L21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N21" s="5" t="s">
         <v>31</v>
@@ -1449,7 +1479,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E22" s="5">
         <v>1</v>
@@ -1462,11 +1492,11 @@
       </c>
       <c r="H22" s="6">
         <f>G18</f>
-        <v>43339</v>
+        <v>43318</v>
       </c>
       <c r="I22" s="6">
         <f>H22+G22</f>
-        <v>43340</v>
+        <v>43319</v>
       </c>
       <c r="J22" s="5">
         <v>2</v>
@@ -1476,15 +1506,15 @@
       </c>
       <c r="L22" s="5">
         <f>$C$18</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M22" s="14">
-        <f>(G22/$T$18)*100</f>
-        <v>6.666666666666667</v>
+        <f>(G22/$T$18)</f>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="N22" s="14">
         <f>IF(J22=2,M22/100,0)</f>
-        <v>6.6666666666666666E-2</v>
+        <v>6.6666666666666664E-4</v>
       </c>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.25">
@@ -1492,7 +1522,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E23" s="5">
         <v>2</v>
@@ -1505,28 +1535,28 @@
       </c>
       <c r="H23" s="6">
         <f>I22</f>
-        <v>43340</v>
+        <v>43319</v>
       </c>
       <c r="I23" s="6">
-        <f t="shared" ref="I23:I26" si="0">H23+G23</f>
-        <v>43342</v>
+        <f>H23+G23</f>
+        <v>43321</v>
       </c>
       <c r="J23" s="5">
         <v>2</v>
       </c>
       <c r="K23" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L23" s="5">
-        <f t="shared" ref="L23:L26" si="1">$C$18</f>
-        <v>1</v>
+        <f t="shared" ref="L23:L26" si="0">$C$18</f>
+        <v>6</v>
       </c>
       <c r="M23" s="14">
         <f>G23/$T$18</f>
         <v>0.13333333333333333</v>
       </c>
       <c r="N23" s="14">
-        <f t="shared" ref="N23:N26" si="2">IF(J23=2,M23/100,0)</f>
+        <f>IF(J23=2,M23/100,0)</f>
         <v>1.3333333333333333E-3</v>
       </c>
     </row>
@@ -1535,7 +1565,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E24" s="5">
         <v>3</v>
@@ -1544,33 +1574,33 @@
         <v>1</v>
       </c>
       <c r="G24" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H24" s="6">
-        <f t="shared" ref="H24:H26" si="3">I23</f>
-        <v>43342</v>
+        <f>I23</f>
+        <v>43321</v>
       </c>
       <c r="I24" s="6">
+        <f>H24+G24</f>
+        <v>43326</v>
+      </c>
+      <c r="J24" s="5">
+        <v>2</v>
+      </c>
+      <c r="K24" s="5">
+        <v>9</v>
+      </c>
+      <c r="L24" s="5">
         <f t="shared" si="0"/>
-        <v>43345</v>
-      </c>
-      <c r="J24" s="5">
-        <v>3</v>
-      </c>
-      <c r="K24" s="5">
-        <v>4</v>
-      </c>
-      <c r="L24" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M24" s="14">
-        <f t="shared" ref="M24:M26" si="4">G24/$T$18</f>
-        <v>0.2</v>
+        <f>G24/$T$18</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N24" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>IF(J24=2,M24/100,0)</f>
+        <v>3.3333333333333331E-3</v>
       </c>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.25">
@@ -1578,7 +1608,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E25" s="5">
         <v>4</v>
@@ -1590,30 +1620,30 @@
         <v>4</v>
       </c>
       <c r="H25" s="6">
-        <f t="shared" si="3"/>
-        <v>43345</v>
+        <f>I24</f>
+        <v>43326</v>
       </c>
       <c r="I25" s="6">
-        <f t="shared" si="0"/>
-        <v>43349</v>
+        <f>H25+G25</f>
+        <v>43330</v>
       </c>
       <c r="J25" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K25" s="5">
         <v>5</v>
       </c>
       <c r="L25" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="M25" s="14">
-        <f t="shared" si="4"/>
+        <f>G25/$T$18</f>
         <v>0.26666666666666666</v>
       </c>
       <c r="N25" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>IF(J25=2,M25/100,0)</f>
+        <v>2.6666666666666666E-3</v>
       </c>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.25">
@@ -1621,7 +1651,7 @@
         <v>5</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E26" s="5">
         <v>5</v>
@@ -1630,33 +1660,33 @@
         <v>1</v>
       </c>
       <c r="G26" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H26" s="6">
-        <f t="shared" si="3"/>
-        <v>43349</v>
+        <f>I25</f>
+        <v>43330</v>
       </c>
       <c r="I26" s="6">
+        <f>H26+G26</f>
+        <v>43333</v>
+      </c>
+      <c r="J26" s="5">
+        <v>2</v>
+      </c>
+      <c r="K26" s="5">
+        <v>10</v>
+      </c>
+      <c r="L26" s="5">
         <f t="shared" si="0"/>
-        <v>43354</v>
-      </c>
-      <c r="J26" s="5">
-        <v>3</v>
-      </c>
-      <c r="K26" s="5">
         <v>6</v>
       </c>
-      <c r="L26" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="M26" s="14">
-        <f t="shared" si="4"/>
-        <v>0.33333333333333331</v>
+        <f>G26/$T$18</f>
+        <v>0.2</v>
       </c>
       <c r="N26" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>IF(J26=2,M26/100,0)</f>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.25">
@@ -1675,7 +1705,7 @@
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="G28" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N28" s="15"/>
     </row>
@@ -1687,7 +1717,7 @@
         <v>13</v>
       </c>
       <c r="D29" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E29" t="s">
         <v>27</v>
@@ -1702,20 +1732,21 @@
         <v>24</v>
       </c>
       <c r="I29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C30" s="5">
-        <v>1</v>
+        <f>$C$18</f>
+        <v>6</v>
       </c>
       <c r="D30" s="5">
         <f>$C$18</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E30" s="9">
-        <f>G18</f>
-        <v>43339</v>
+        <f>$G$18</f>
+        <v>43318</v>
       </c>
       <c r="F30" s="5">
         <f>$J$18</f>
@@ -1726,7 +1757,7 @@
       </c>
       <c r="H30" s="5">
         <f>$N$18</f>
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.25">
@@ -1739,36 +1770,36 @@
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="J32" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C33" t="s">
         <v>13</v>
       </c>
       <c r="D33" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" t="s">
         <v>74</v>
       </c>
-      <c r="E33" t="s">
-        <v>75</v>
-      </c>
-      <c r="F33" t="s">
-        <v>76</v>
-      </c>
-      <c r="G33" t="s">
-        <v>77</v>
-      </c>
       <c r="H33" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.25">
@@ -1777,13 +1808,13 @@
       </c>
       <c r="D34">
         <f>$C$30</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
       <c r="F34">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G34">
         <v>6</v>
@@ -1792,11 +1823,12 @@
         <v>2</v>
       </c>
       <c r="I34">
+        <f>$T$18</f>
         <v>15</v>
       </c>
       <c r="J34" s="2">
         <f>(F34*M3)*I34</f>
-        <v>4500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.25">
@@ -1804,14 +1836,14 @@
         <v>2</v>
       </c>
       <c r="D35" s="17">
-        <f t="shared" ref="D35:D37" si="5">$C$30</f>
-        <v>1</v>
+        <f t="shared" ref="D35:D37" si="1">$C$30</f>
+        <v>6</v>
       </c>
       <c r="E35">
         <v>3</v>
       </c>
       <c r="F35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G35">
         <v>3</v>
@@ -1819,12 +1851,13 @@
       <c r="H35">
         <v>2</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="17">
+        <f t="shared" ref="I35:I36" si="2">$T$18</f>
         <v>15</v>
       </c>
       <c r="J35" s="2">
         <f>(F35*M5)*I35</f>
-        <v>2250</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.25">
@@ -1832,14 +1865,14 @@
         <v>3</v>
       </c>
       <c r="D36" s="17">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="E36">
         <v>9</v>
       </c>
       <c r="F36">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G36">
         <v>6</v>
@@ -1847,12 +1880,13 @@
       <c r="H36">
         <v>2</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="17">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="J36" s="2">
         <f>(F36*M11)*I36</f>
-        <v>1350</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.25">
@@ -1860,8 +1894,8 @@
         <v>4</v>
       </c>
       <c r="D37" s="17">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="E37">
         <v>8</v>
@@ -1891,12 +1925,12 @@
       <c r="F41" s="17"/>
       <c r="G41" s="17"/>
       <c r="H41" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I41" s="17"/>
       <c r="J41" s="17"/>
       <c r="K41" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L41" s="17"/>
       <c r="M41" s="17"/>
@@ -1907,7 +1941,7 @@
       <c r="R41" s="17"/>
       <c r="S41" s="17"/>
       <c r="T41" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="U41" s="17"/>
       <c r="V41" s="17"/>
@@ -1915,7 +1949,7 @@
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B42" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C42" s="17" t="s">
         <v>13</v>
@@ -1927,7 +1961,7 @@
         <v>16</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G42" s="17" t="s">
         <v>17</v>
@@ -1987,7 +2021,7 @@
         <v>4</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E43" s="13">
         <v>7000</v>
@@ -2025,7 +2059,7 @@
         <v>1</v>
       </c>
       <c r="P43" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="Q43" s="9">
         <f>G43</f>
@@ -2047,10 +2081,10 @@
         <v>0.22222222222222221</v>
       </c>
       <c r="V43" s="17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="W43" s="17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.25">
@@ -2087,7 +2121,7 @@
       <c r="H45" s="17"/>
       <c r="I45" s="17"/>
       <c r="J45" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K45" s="17"/>
       <c r="L45" s="17"/>
@@ -2114,7 +2148,7 @@
         <v>14</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>29</v>
@@ -2135,10 +2169,10 @@
         <v>24</v>
       </c>
       <c r="L46" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N46" s="5" t="s">
         <v>31</v>
@@ -2159,7 +2193,7 @@
         <v>1</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E47" s="5">
         <v>1</v>
@@ -2212,7 +2246,7 @@
         <v>2</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E48" s="5">
         <v>2</v>
@@ -2228,7 +2262,7 @@
         <v>43328</v>
       </c>
       <c r="I48" s="6">
-        <f t="shared" ref="I48:I51" si="6">H48+G48</f>
+        <f t="shared" ref="I48:I51" si="3">H48+G48</f>
         <v>43331</v>
       </c>
       <c r="J48" s="5">
@@ -2238,15 +2272,15 @@
         <v>3</v>
       </c>
       <c r="L48" s="5">
-        <f t="shared" ref="L48:L51" si="7">$C$43</f>
+        <f t="shared" ref="L48:L51" si="4">$C$43</f>
         <v>4</v>
       </c>
       <c r="M48" s="14">
-        <f t="shared" ref="M48:M51" si="8">(G48/$T$43)</f>
+        <f t="shared" ref="M48:M51" si="5">(G48/$T$43)</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="N48" s="14">
-        <f t="shared" ref="N48:N51" si="9">IF(J48=2,M48,0)</f>
+        <f t="shared" ref="N48:N51" si="6">IF(J48=2,M48,0)</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="O48" s="17"/>
@@ -2265,7 +2299,7 @@
         <v>3</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E49" s="5">
         <v>3</v>
@@ -2277,11 +2311,11 @@
         <v>4</v>
       </c>
       <c r="H49" s="6">
-        <f t="shared" ref="H49:H51" si="10">I48</f>
+        <f t="shared" ref="H49:H51" si="7">I48</f>
         <v>43331</v>
       </c>
       <c r="I49" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>43335</v>
       </c>
       <c r="J49" s="5">
@@ -2291,15 +2325,15 @@
         <v>4</v>
       </c>
       <c r="L49" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="M49" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="N49" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O49" s="17"/>
@@ -2318,7 +2352,7 @@
         <v>4</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E50" s="5">
         <v>4</v>
@@ -2330,11 +2364,11 @@
         <v>8</v>
       </c>
       <c r="H50" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>43335</v>
       </c>
       <c r="I50" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>43343</v>
       </c>
       <c r="J50" s="5">
@@ -2344,15 +2378,15 @@
         <v>5</v>
       </c>
       <c r="L50" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="M50" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="N50" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O50" s="17"/>
@@ -2371,7 +2405,7 @@
         <v>5</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E51" s="5">
         <v>5</v>
@@ -2383,11 +2417,11 @@
         <v>2</v>
       </c>
       <c r="H51" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>43343</v>
       </c>
       <c r="I51" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>43345</v>
       </c>
       <c r="J51" s="5">
@@ -2397,15 +2431,15 @@
         <v>6</v>
       </c>
       <c r="L51" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="M51" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="N51" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O51" s="17"/>
@@ -2449,7 +2483,7 @@
       <c r="E53" s="17"/>
       <c r="F53" s="17"/>
       <c r="G53" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H53" s="17"/>
       <c r="I53" s="17"/>
@@ -2476,7 +2510,7 @@
         <v>13</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E54" s="17" t="s">
         <v>27</v>
@@ -2491,7 +2525,7 @@
         <v>24</v>
       </c>
       <c r="I54" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J54" s="17"/>
       <c r="K54" s="17"/>
@@ -2580,7 +2614,7 @@
       <c r="H57" s="17"/>
       <c r="I57" s="17"/>
       <c r="J57" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="K57" s="17"/>
       <c r="L57" s="17"/>
@@ -2598,31 +2632,31 @@
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B58" s="17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C58" s="17" t="s">
         <v>13</v>
       </c>
       <c r="D58" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E58" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="G58" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="E58" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="F58" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="G58" s="17" t="s">
-        <v>77</v>
-      </c>
       <c r="H58" s="17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I58" s="17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K58" s="17"/>
       <c r="L58" s="17"/>
@@ -2686,7 +2720,7 @@
         <v>2</v>
       </c>
       <c r="D60" s="17">
-        <f t="shared" ref="D60:D62" si="11">$C$55</f>
+        <f t="shared" ref="D60:D62" si="8">$C$55</f>
         <v>4</v>
       </c>
       <c r="E60" s="17">
@@ -2728,7 +2762,7 @@
         <v>3</v>
       </c>
       <c r="D61" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="E61" s="17">
@@ -2770,7 +2804,7 @@
         <v>4</v>
       </c>
       <c r="D62" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="E62" s="17">
@@ -2882,22 +2916,22 @@
         <v>30</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3057,20 +3091,20 @@
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="45" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="18" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -3104,7 +3138,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G4" s="25">
         <f>IF(F4="C",E4/$E$3,0)</f>
@@ -3124,7 +3158,7 @@
         <v>0.125</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G5" s="25">
         <f t="shared" ref="G5:G13" si="1">IF(F5="C",E5/$E$3,0)</f>
@@ -3144,7 +3178,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G6" s="25">
         <f t="shared" si="1"/>
@@ -3164,7 +3198,7 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G7" s="25">
         <f t="shared" si="1"/>
@@ -3184,7 +3218,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G8" s="25">
         <f t="shared" si="1"/>
@@ -3204,7 +3238,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G9" s="25">
         <f t="shared" si="1"/>
@@ -3224,7 +3258,7 @@
         <v>9.5833333333333326E-2</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G10" s="25">
         <f t="shared" si="1"/>
@@ -3244,7 +3278,7 @@
         <v>7.0833333333333331E-2</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G11" s="25">
         <f t="shared" si="1"/>
@@ -3264,7 +3298,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G12" s="25">
         <f t="shared" si="1"/>
@@ -3284,7 +3318,7 @@
         <v>0.125</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G13" s="30">
         <f t="shared" si="1"/>
@@ -3301,25 +3335,25 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="45" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C15" s="46"/>
       <c r="D15" s="18" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C16" s="22"/>
       <c r="D16" s="23">
@@ -3338,7 +3372,7 @@
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="21"/>
       <c r="C17" s="22" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D17" s="23">
         <v>2</v>
@@ -3348,7 +3382,7 @@
         <v>0.125</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G17" s="25">
         <f>IF(F17="C",E17/$E$16,0)</f>
@@ -3358,7 +3392,7 @@
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="21"/>
       <c r="C18" s="22" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D18" s="23">
         <v>0.5</v>
@@ -3368,7 +3402,7 @@
         <v>3.125E-2</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G18" s="25">
         <f t="shared" ref="G18:G22" si="3">IF(F18="C",E18/$E$16,0)</f>
@@ -3378,7 +3412,7 @@
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="21"/>
       <c r="C19" s="22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D19" s="23">
         <v>1.5</v>
@@ -3388,7 +3422,7 @@
         <v>9.375E-2</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G19" s="25">
         <f t="shared" si="3"/>
@@ -3398,7 +3432,7 @@
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="21"/>
       <c r="C20" s="22" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D20" s="23">
         <v>5</v>
@@ -3408,7 +3442,7 @@
         <v>0.3125</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G20" s="25">
         <f t="shared" si="3"/>
@@ -3418,7 +3452,7 @@
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="21"/>
       <c r="C21" s="22" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D21" s="23">
         <v>3</v>
@@ -3428,7 +3462,7 @@
         <v>0.1875</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G21" s="25">
         <f t="shared" si="3"/>
@@ -3438,7 +3472,7 @@
     <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="26"/>
       <c r="C22" s="27" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D22" s="28">
         <v>4</v>
@@ -3448,7 +3482,7 @@
         <v>0.25</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G22" s="30">
         <f t="shared" si="3"/>

</xml_diff>